<commit_message>
doing 5-6 lab java(23mar 2023)
</commit_message>
<xml_diff>
--- a/Artificial Intelegense/file.xlsx
+++ b/Artificial Intelegense/file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vita2\IdeaProjects\Artificial Intelegense\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA83EE0-E9D1-405D-99AD-3AA03EE59960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0A64A6-2A4D-4F11-BDDA-8A75328D72F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14790" yWindow="1920" windowWidth="9900" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -340,7 +340,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>